<commit_message>
[ADD] support for Google Meet and update README
</commit_message>
<xml_diff>
--- a/meetings.xlsx
+++ b/meetings.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5844"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="meetings" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>meeting_id</t>
   </si>
@@ -35,7 +35,16 @@
     <t>time</t>
   </si>
   <si>
-    <t>user</t>
+    <t>type</t>
+  </si>
+  <si>
+    <t>zoom</t>
+  </si>
+  <si>
+    <t>google_meet</t>
+  </si>
+  <si>
+    <t>https://meet.google.com/url_to_your_metting</t>
   </si>
   <si>
     <t>juan</t>
@@ -45,13 +54,19 @@
   </si>
   <si>
     <t>sofia</t>
+  </si>
+  <si>
+    <t>raul</t>
+  </si>
+  <si>
+    <t>title</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -75,6 +90,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -93,10 +116,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -109,8 +133,12 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -389,20 +417,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.6640625" customWidth="1"/>
-    <col min="2" max="2" width="21.33203125" customWidth="1"/>
+    <col min="1" max="1" width="41" customWidth="1"/>
+    <col min="2" max="2" width="24.33203125" customWidth="1"/>
     <col min="3" max="3" width="20.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -415,8 +443,11 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>1234567890</v>
       </c>
@@ -429,22 +460,26 @@
       <c r="D2" t="s">
         <v>4</v>
       </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="3">
-        <v>1234567890</v>
-      </c>
-      <c r="B3" s="3">
-        <v>123456</v>
-      </c>
+    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="3"/>
       <c r="C3" s="4">
-        <v>0.4368055555555555</v>
+        <v>0.50277777777777777</v>
       </c>
       <c r="D3" t="s">
         <v>5</v>
       </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>1234567890</v>
       </c>
@@ -452,17 +487,39 @@
         <v>123456</v>
       </c>
       <c r="C4" s="4">
-        <v>0.47847222222222202</v>
+        <v>0.54444444444444395</v>
       </c>
       <c r="D4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
         <v>6</v>
       </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="4">
+        <v>0.75277777777777777</v>
+      </c>
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B10" s="5"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A3" r:id="rId1"/>
+    <hyperlink ref="A5" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[ADD] Drop-down lists for days and types in the Excel sheet
</commit_message>
<xml_diff>
--- a/meetings.xlsx
+++ b/meetings.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>meeting_id</t>
   </si>
@@ -53,13 +53,16 @@
     <t>pedro</t>
   </si>
   <si>
-    <t>sofia</t>
-  </si>
-  <si>
-    <t>raul</t>
-  </si>
-  <si>
     <t>title</t>
+  </si>
+  <si>
+    <t>day</t>
+  </si>
+  <si>
+    <t>monday</t>
+  </si>
+  <si>
+    <t>friday</t>
   </si>
 </sst>
 </file>
@@ -417,20 +420,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
-    <col min="2" max="2" width="24.33203125" customWidth="1"/>
-    <col min="3" max="3" width="20.44140625" customWidth="1"/>
+    <col min="2" max="3" width="24.33203125" customWidth="1"/>
+    <col min="4" max="4" width="23.6640625" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -438,88 +442,101 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>1234567890</v>
       </c>
       <c r="B2" s="3">
         <v>123456</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="4">
         <v>0.43611111111111112</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="3"/>
-      <c r="C3" s="4">
-        <v>0.50277777777777777</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="C3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0.59652777777777777</v>
+      </c>
+      <c r="E3" t="s">
         <v>5</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="3">
-        <v>1234567890</v>
-      </c>
-      <c r="B4" s="3">
-        <v>123456</v>
-      </c>
-      <c r="C4" s="4">
-        <v>0.54444444444444395</v>
-      </c>
-      <c r="D4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
-        <v>6</v>
-      </c>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="4"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="6"/>
       <c r="B5" s="3"/>
-      <c r="C5" s="4">
-        <v>0.75277777777777777</v>
-      </c>
-      <c r="D5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C5" s="3"/>
+      <c r="D5" s="4"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="4"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="6"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="4"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="4"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
     </row>
   </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1048576">
+      <formula1>"monday,tuesday,wednesday,thursday,friday,saturday,sunday"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E1048576">
+      <formula1>"zoom,google_meet"</formula1>
+    </dataValidation>
+  </dataValidations>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1"/>
-    <hyperlink ref="A5" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[ADD] Schedule tasks for today's day of the week only
</commit_message>
<xml_diff>
--- a/meetings.xlsx
+++ b/meetings.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>meeting_id</t>
   </si>
@@ -53,16 +53,13 @@
     <t>pedro</t>
   </si>
   <si>
-    <t>title</t>
-  </si>
-  <si>
     <t>day</t>
   </si>
   <si>
-    <t>monday</t>
-  </si>
-  <si>
     <t>friday</t>
+  </si>
+  <si>
+    <t>user</t>
   </si>
 </sst>
 </file>
@@ -420,73 +417,74 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="41" customWidth="1"/>
-    <col min="2" max="3" width="24.33203125" customWidth="1"/>
-    <col min="4" max="4" width="23.6640625" customWidth="1"/>
+    <col min="1" max="1" width="24.33203125" customWidth="1"/>
+    <col min="2" max="2" width="23.6640625" customWidth="1"/>
+    <col min="3" max="3" width="41" customWidth="1"/>
+    <col min="4" max="4" width="24.33203125" customWidth="1"/>
     <col min="5" max="5" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="3">
-        <v>1234567890</v>
-      </c>
-      <c r="B2" s="3">
-        <v>123456</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="4">
-        <v>0.43611111111111112</v>
-      </c>
+      <c r="A2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="4">
+        <v>0.64722222222222225</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="3"/>
       <c r="E2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="4">
-        <v>0.59652777777777777</v>
+      <c r="A3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="4">
+        <v>0.64722222222222225</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1234567890</v>
+      </c>
+      <c r="D3" s="3">
+        <v>123456</v>
       </c>
       <c r="E3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F3" t="s">
         <v>8</v>
@@ -494,39 +492,33 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="3"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="6"/>
-      <c r="B5" s="3"/>
+      <c r="A5" s="3"/>
+      <c r="B5" s="4"/>
       <c r="C5" s="3"/>
-      <c r="D5" s="4"/>
+      <c r="D5" s="3"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="6"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="6"/>
+      <c r="A7" s="3"/>
+      <c r="B7" s="4"/>
       <c r="C7" s="3"/>
-      <c r="D7" s="4"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="4"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="5"/>
+      <c r="D9" s="5"/>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A1048576">
       <formula1>"monday,tuesday,wednesday,thursday,friday,saturday,sunday"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E1048576">
@@ -534,7 +526,7 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1"/>
+    <hyperlink ref="C2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
[FIX] Get tab  for automatic join
</commit_message>
<xml_diff>
--- a/meetings.xlsx
+++ b/meetings.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\davidharo\PycharmProjects\schedule_zoom\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEEE9716-C895-4303-9FE3-91D2937D7385}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5844"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meetings" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
   <si>
     <t>meeting_id</t>
   </si>
@@ -41,32 +42,62 @@
     <t>zoom</t>
   </si>
   <si>
-    <t>google_meet</t>
-  </si>
-  <si>
-    <t>https://meet.google.com/url_to_your_metting</t>
-  </si>
-  <si>
-    <t>juan</t>
-  </si>
-  <si>
-    <t>pedro</t>
-  </si>
-  <si>
     <t>day</t>
   </si>
   <si>
+    <t>user</t>
+  </si>
+  <si>
+    <t>monday</t>
+  </si>
+  <si>
+    <t>943 835 6448</t>
+  </si>
+  <si>
+    <t>tuesday</t>
+  </si>
+  <si>
+    <t>857 069 3962</t>
+  </si>
+  <si>
+    <t>wednesday</t>
+  </si>
+  <si>
+    <t>650 460 3098</t>
+  </si>
+  <si>
+    <t>David Haro</t>
+  </si>
+  <si>
+    <t>Jesus Rodriguez</t>
+  </si>
+  <si>
+    <t>Brenda Carranco</t>
+  </si>
+  <si>
+    <t>saturday</t>
+  </si>
+  <si>
+    <t>thursday</t>
+  </si>
+  <si>
+    <t>055902</t>
+  </si>
+  <si>
+    <t>Miguel Alvarez</t>
+  </si>
+  <si>
     <t>friday</t>
   </si>
   <si>
-    <t>user</t>
+    <t>All Hands Meeting</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -90,14 +121,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -116,29 +139,37 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -416,119 +447,174 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.33203125" customWidth="1"/>
-    <col min="2" max="2" width="23.6640625" customWidth="1"/>
-    <col min="3" max="3" width="41" customWidth="1"/>
-    <col min="4" max="4" width="24.33203125" customWidth="1"/>
-    <col min="5" max="5" width="20.6640625" customWidth="1"/>
+    <col min="1" max="1" width="24.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="23.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="41" style="1" customWidth="1"/>
+    <col min="4" max="4" width="24.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.77734375" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="11.5546875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="1" t="s">
+      <c r="A1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="4">
-        <v>0.64722222222222225</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="3"/>
-      <c r="E2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="A2" s="5" t="s">
         <v>7</v>
+      </c>
+      <c r="B2" s="6">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="5">
+        <v>123456</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="6">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="4">
-        <v>0.64722222222222225</v>
-      </c>
-      <c r="C3" s="3">
-        <v>1234567890</v>
-      </c>
-      <c r="D3" s="3">
-        <v>123456</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="D3" s="5">
+        <v>536994</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F3" t="s">
-        <v>8</v>
+      <c r="F3" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="3"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="3"/>
+      <c r="A4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="6">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="5">
+        <v>123456</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="3"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
+      <c r="A5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="6">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="5">
+        <v>123456</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="3"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="6"/>
+      <c r="A6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="7">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="C6" s="1">
+        <v>8484246662</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="3"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="3"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="5"/>
-      <c r="D9" s="5"/>
+      <c r="A7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="7">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C7" s="1">
+        <v>7544068640</v>
+      </c>
+      <c r="D7" s="3">
+        <v>652801</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"monday,tuesday,wednesday,thursday,friday,saturday,sunday"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E1048576" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"zoom,google_meet"</formula1>
     </dataValidation>
   </dataValidations>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>